<commit_message>
Attempting to merge all files and directories, branch seems to have run completely isolated to master.
</commit_message>
<xml_diff>
--- a/excel_data/Vessel_data.xlsx
+++ b/excel_data/Vessel_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Checkouts\Terminal_optimization\excel_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D945B4A7-3F98-4A68-A1AC-1E7DA2E81FDF}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFC7CE63-E8E9-4675-AC29-5521144D7F21}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13365" activeTab="1" xr2:uid="{B7B37447-70F1-4FBA-B5DB-2FBF99E1D180}"/>
   </bookViews>
@@ -468,10 +468,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21DD3DE0-F388-48A7-B07F-F7B0E1C25327}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:R29"/>
+  <dimension ref="A1:P29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+      <selection activeCell="Q5" sqref="Q5:R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,7 +482,7 @@
     <col min="11" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -532,7 +532,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1991</v>
       </c>
@@ -584,7 +584,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1992</v>
       </c>
@@ -636,7 +636,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1993</v>
       </c>
@@ -688,7 +688,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1994</v>
       </c>
@@ -739,15 +739,8 @@
       <c r="P5" t="s">
         <v>6</v>
       </c>
-      <c r="Q5">
-        <v>11.4</v>
-      </c>
-      <c r="R5">
-        <f>0.66*Q5+0.33*Q6</f>
-        <v>11.715</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1995</v>
       </c>
@@ -798,11 +791,8 @@
       <c r="P6" t="s">
         <v>7</v>
       </c>
-      <c r="Q6">
-        <v>12.7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1996</v>
       </c>
@@ -854,7 +844,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1997</v>
       </c>
@@ -906,7 +896,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1998</v>
       </c>
@@ -958,7 +948,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1999</v>
       </c>
@@ -1010,7 +1000,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2000</v>
       </c>
@@ -1062,7 +1052,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2001</v>
       </c>
@@ -1108,7 +1098,7 @@
         <v>51115.348837209305</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2002</v>
       </c>
@@ -1154,7 +1144,7 @@
         <v>52346.111719605695</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2003</v>
       </c>
@@ -1200,7 +1190,7 @@
         <v>53079.906204906205</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2004</v>
       </c>
@@ -1246,7 +1236,7 @@
         <v>53894.840207105874</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2005</v>
       </c>
@@ -1901,7 +1891,7 @@
   <dimension ref="A1:U11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>